<commit_message>
Copied the v1.3 into v1.4 folder, and noted down v1.3 LED and buttons locations
</commit_message>
<xml_diff>
--- a/Projects/IR Hub for RPi v1.4/HaHub-order.xlsx
+++ b/Projects/IR Hub for RPi v1.4/HaHub-order.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
   <si>
     <t>Value</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>Ordered</t>
+  </si>
+  <si>
+    <t>for each board</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="ORDER??" dataDxfId="0">
+    <tableColumn id="1" name="ORDER??" dataDxfId="1">
       <calculatedColumnFormula>IF(D2&gt;(C2+B2),"ORDER","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Ordered" dataDxfId="1"/>
+    <tableColumn id="12" name="Ordered" dataDxfId="0"/>
     <tableColumn id="2" name="Available"/>
     <tableColumn id="3" name="Required"/>
     <tableColumn id="4" name="Value"/>
@@ -763,11 +766,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -822,188 +823,249 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" s="3" customFormat="1">
       <c r="A2" s="16" t="str">
         <f t="shared" ref="A2:A25" si="0">IF(D2&gt;(C2+B2),"ORDER","")</f>
         <v/>
       </c>
       <c r="B2" s="16"/>
-      <c r="C2">
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="E2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="3">
+        <v>46315</v>
+      </c>
+      <c r="K2" s="9">
+        <v>1.9E-2</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1">
       <c r="A3" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B3" s="16"/>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1">
       <c r="A4" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B4" s="16"/>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1">
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1">
       <c r="A5" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="16"/>
+      <c r="C5" s="4">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1">
+      <c r="A6" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="2">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="3">
-        <v>46315</v>
-      </c>
-      <c r="K5" s="9">
-        <v>1.9E-2</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1">
-      <c r="A6" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B6" s="16">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1">
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1558</v>
+      </c>
+      <c r="K6" s="11">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1">
       <c r="A7" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B7" s="16"/>
-      <c r="C7" s="3">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" s="4" customFormat="1">
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2513</v>
+      </c>
+      <c r="K7" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1">
       <c r="A8" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B8" s="16">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" s="2" customFormat="1">
+      <c r="B8" s="16"/>
+      <c r="C8" s="1">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5587</v>
+      </c>
+      <c r="K8" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1">
       <c r="A9" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B9" s="16">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1558</v>
-      </c>
-      <c r="K9" s="11">
-        <v>1.6E-2</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>12</v>
+      <c r="B9" s="16"/>
+      <c r="C9" s="1">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="1">
+        <v>6062</v>
+      </c>
+      <c r="K9" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1">
@@ -1013,34 +1075,34 @@
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J10" s="1">
-        <v>2513</v>
+        <v>10313</v>
       </c>
       <c r="K10" s="12">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1">
@@ -1050,34 +1112,34 @@
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="1">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="J11" s="1">
-        <v>5587</v>
+        <v>3631</v>
       </c>
       <c r="K11" s="12">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1">
@@ -1087,145 +1149,136 @@
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="1">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="J12" s="1">
-        <v>6062</v>
+        <v>2145</v>
       </c>
       <c r="K12" s="12">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1">
       <c r="A13" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="16"/>
+      <c r="C13" s="5">
+        <v>11</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="5">
+        <v>10342</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0.126</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="5" customFormat="1">
+      <c r="A14" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="5">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="5">
+        <v>4900</v>
+      </c>
+      <c r="K14" s="13">
+        <v>0.126</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="5" customFormat="1">
+      <c r="A15" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="1">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="1">
-        <v>10313</v>
-      </c>
-      <c r="K13" s="12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1">
-      <c r="A14" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B14" s="16">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="1">
-        <v>3631</v>
-      </c>
-      <c r="K14" s="12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1">
-      <c r="A15" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B15" s="16">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J15" s="1">
-        <v>2145</v>
-      </c>
-      <c r="K15" s="12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>63</v>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="5">
+        <v>7488</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0.126</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1">
@@ -1235,270 +1288,221 @@
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="5">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D16" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="J16" s="5">
-        <v>10342</v>
+        <v>2943</v>
       </c>
       <c r="K16" s="13">
         <v>0.126</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="5" customFormat="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="7" customFormat="1">
       <c r="A17" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>ORDER</v>
+        <v/>
       </c>
       <c r="B17" s="16"/>
-      <c r="C17" s="5">
-        <v>8</v>
-      </c>
-      <c r="D17" s="5">
-        <v>9</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="5">
-        <v>4900</v>
-      </c>
-      <c r="K17" s="13">
-        <v>0.126</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="5" customFormat="1">
+      <c r="C17" s="7">
+        <v>10</v>
+      </c>
+      <c r="D17" s="7">
+        <v>2</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="7">
+        <v>2987</v>
+      </c>
+      <c r="K17" s="14">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="7" customFormat="1">
       <c r="A18" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B18" s="16">
-        <v>10</v>
-      </c>
-      <c r="D18" s="5">
+      <c r="B18" s="16"/>
+      <c r="C18" s="7">
         <v>3</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="5">
-        <v>7488</v>
-      </c>
-      <c r="K18" s="13">
-        <v>0.126</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="5" customFormat="1">
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="7">
+        <v>6109</v>
+      </c>
+      <c r="K18" s="14">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="6" customFormat="1">
       <c r="A19" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B19" s="16"/>
-      <c r="C19" s="5">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5">
-        <v>3</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="5">
-        <v>2943</v>
-      </c>
-      <c r="K19" s="13">
-        <v>0.126</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="7" customFormat="1">
+      <c r="C19" s="6">
+        <v>14</v>
+      </c>
+      <c r="D19" s="6">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="6">
+        <v>404</v>
+      </c>
+      <c r="K19" s="15">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="6" customFormat="1">
       <c r="A20" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B20" s="16"/>
-      <c r="C20" s="7">
-        <v>10</v>
-      </c>
-      <c r="D20" s="7">
-        <v>6</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="7">
-        <v>2987</v>
-      </c>
-      <c r="K20" s="14">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="7" customFormat="1">
+      <c r="C20" s="6">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0</v>
+      </c>
+      <c r="K20" s="15">
+        <v>0.104</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D21&gt;(C21+B21),"ORDER","")</f>
         <v/>
       </c>
       <c r="B21" s="16"/>
-      <c r="C21" s="7">
-        <v>3</v>
-      </c>
-      <c r="D21" s="7">
-        <v>3</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="7">
-        <v>6109</v>
-      </c>
-      <c r="K21" s="14">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="6" customFormat="1">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D22&gt;(C22+B22),"ORDER","")</f>
         <v/>
       </c>
       <c r="B22" s="16"/>
-      <c r="C22" s="6">
-        <v>14</v>
-      </c>
-      <c r="D22" s="6">
-        <v>12</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J22" s="6">
-        <v>404</v>
-      </c>
-      <c r="K22" s="15">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="6" customFormat="1">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B23" s="16">
-        <v>6</v>
-      </c>
-      <c r="C23" s="6">
-        <v>1</v>
-      </c>
-      <c r="D23" s="6">
-        <v>6</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="J23" s="6">
-        <v>0</v>
-      </c>
-      <c r="K23" s="15">
-        <v>0.104</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>83</v>
+        <f>IF(D23&gt;(C23+B23),"ORDER","")</f>
+        <v/>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1537,6 +1541,11 @@
       </c>
       <c r="L25" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="D27" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>